<commit_message>
Add our template for plasma
This is very similar to the "Gates" plasma template, but also includes columns for drug dosage and dose interval, so these data can be summarized into the format need for the efficacy summary dataframe format being used by groups 2 and 3.
</commit_message>
<xml_diff>
--- a/our_templates/Our_Template_Plasma R.xlsx
+++ b/our_templates/Our_Template_Plasma R.xlsx
@@ -1486,8 +1486,8 @@
   </sheetPr>
   <dimension ref="A1:N300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B300"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>